<commit_message>
Corrected part no for Micro USB on switch network
</commit_message>
<xml_diff>
--- a/doc/PCB/BOM_Example.xlsx
+++ b/doc/PCB/BOM_Example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="SwitchBoard" localSheetId="0">BOM!$A$1:$I$74</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -559,8 +559,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,6 +712,13 @@
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1056,7 +1063,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1083,6 +1090,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1133,6 +1141,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1185,7 +1196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1220,7 +1231,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,9 +1442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H72:H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,8 +3358,8 @@
       <c r="F74" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G74" s="8">
-        <v>2443114</v>
+      <c r="G74" s="12">
+        <v>2293836</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>